<commit_message>
add new function to search for potential ssn information and update clean data dictionary
</commit_message>
<xml_diff>
--- a/2-Config-Files/cds_config/UI-database mappings_v2.xlsx
+++ b/2-Config-Files/cds_config/UI-database mappings_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muelleras\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangf6/Documents/cds_v1.2/2-Config-Files/cds_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7200A2E4-F6DA-4E76-BB23-323597DBF633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC19559-5DD8-F145-8B04-7E4102E2969C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="123">
   <si>
     <t>Facet filters</t>
   </si>
@@ -427,6 +427,12 @@
   </si>
   <si>
     <t>primary_diagnosis</t>
+  </si>
+  <si>
+    <t>genomic_info.library_source</t>
+  </si>
+  <si>
+    <t>Study Access</t>
   </si>
 </sst>
 </file>
@@ -796,23 +802,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C948E4-1DF0-6249-BEB1-83F763634681}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.125" customWidth="1"/>
-    <col min="3" max="3" width="30.625" customWidth="1"/>
-    <col min="4" max="4" width="42.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.125" customWidth="1"/>
-    <col min="6" max="6" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -832,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -853,7 +859,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -874,7 +880,7 @@
         <v>primary_diagnosis</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -895,7 +901,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -916,7 +922,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -937,7 +943,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -958,7 +964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -979,7 +985,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1000,7 +1006,7 @@
         <v>experimental_strategy_and_data_subtypes</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>experimental_strategy_and_data_subtypes</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>file_name</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -1063,7 +1069,7 @@
         <v>file_name</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>file_type</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -1105,7 +1111,7 @@
         <v>file_type</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>file_type</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>109</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>file_type</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>instrument_model</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>library_layout</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1200,17 +1206,17 @@
         <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="E19" t="str" cm="1">
         <f t="array" ref="E19:F19">_xlfn.TEXTSPLIT(D19, ".")</f>
         <v>genomic_info</v>
       </c>
       <c r="F19" t="str">
-        <v>library_layout</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>library_source</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>library_selection</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>library_strategy</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1273,7 +1279,7 @@
         <v>platform</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>reference_genome_assembly</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1315,7 +1321,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -1441,7 +1447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>109</v>
       </c>
@@ -1462,7 +1468,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1483,7 +1489,7 @@
         <v>gender</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>gender</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -1525,7 +1531,7 @@
         <v>gender</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -1546,7 +1552,7 @@
         <v>gender</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>participant_id</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>participant_id</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>participant_id</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>109</v>
       </c>
@@ -1630,7 +1636,7 @@
         <v>participant_id</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>program_acronym</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -1672,7 +1678,7 @@
         <v>program_acronym</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>program_external_url</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>program_name</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>program_name</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>program_short_description</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -1777,7 +1783,7 @@
         <v>sample_id</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>sample_id</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>sample_id</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -1924,7 +1930,7 @@
         <v>sample_id</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>sample_tumor_status</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>sample_tumor_status</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>sample_tumor_status</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>sample_tumor_status</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>sample_type</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -2050,7 +2056,7 @@
         <v>sample_type</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>90</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -2113,7 +2119,7 @@
         <v>data_access_level</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -2134,7 +2140,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2176,7 +2182,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>109</v>
       </c>
@@ -2260,7 +2266,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2281,7 +2287,7 @@
         <v>study_data_types</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>study_data_types</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>85</v>
       </c>
@@ -2323,7 +2329,7 @@
         <v>study_data_types</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>109</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>study_data_types</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>study_description</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>109</v>
       </c>
@@ -2386,7 +2392,7 @@
         <v>study_description</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>109</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>study_external_url</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2470,7 +2476,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2491,7 +2497,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2533,7 +2539,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>109</v>
       </c>
@@ -2552,6 +2558,26 @@
       </c>
       <c r="F83" t="str">
         <v>study_name</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>122</v>
+      </c>
+      <c r="B84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" t="s">
+        <v>101</v>
+      </c>
+      <c r="D84" t="s">
+        <v>38</v>
+      </c>
+      <c r="E84" t="s">
+        <v>39</v>
+      </c>
+      <c r="F84" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2573,14 +2599,14 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2591,7 +2617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2603,7 +2629,7 @@
         <v>primary_site</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2615,7 +2641,7 @@
         <v>file_name</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2627,7 +2653,7 @@
         <v>file_type</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -2639,7 +2665,7 @@
         <v>experimental_strategy_and_data_subtypes</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -2650,7 +2676,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2662,7 +2688,7 @@
         <v>gender</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -2674,7 +2700,7 @@
         <v>participant_id</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2686,7 +2712,7 @@
         <v>program_acronym</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2698,7 +2724,7 @@
         <v>program_name</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2710,7 +2736,7 @@
         <v>sample_id</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2722,7 +2748,7 @@
         <v>sample_tumor_status</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2734,7 +2760,7 @@
         <v>sample_type</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2746,7 +2772,7 @@
         <v>data_access_level</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2758,7 +2784,7 @@
         <v>phs_accession</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2770,7 +2796,7 @@
         <v>study_data_types</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2782,7 +2808,7 @@
         <v>study_name</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2793,7 +2819,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -2822,13 +2848,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
@@ -2836,7 +2862,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>108</v>
       </c>
@@ -2844,7 +2870,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>45036</v>
       </c>
@@ -2852,7 +2878,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>45040</v>
       </c>

</xml_diff>

<commit_message>
Update the raw data dictionary
</commit_message>
<xml_diff>
--- a/2-Config-Files/cds_config/UI-database mappings_v2.xlsx
+++ b/2-Config-Files/cds_config/UI-database mappings_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangf6/Documents/cds_v1.2/2-Config-Files/cds_config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangf6/Documents/cds-etl/2-Config-Files/cds_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC19559-5DD8-F145-8B04-7E4102E2969C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E85D267-2D7C-4A4E-9872-5486FB8C0E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="53700" windowHeight="21140" activeTab="2" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="132">
   <si>
     <t>Facet filters</t>
   </si>
@@ -433,13 +433,40 @@
   </si>
   <si>
     <t>Study Access</t>
+  </si>
+  <si>
+    <t>File MD5</t>
+  </si>
+  <si>
+    <t>file.md5sum</t>
+  </si>
+  <si>
+    <t>md5sum</t>
+  </si>
+  <si>
+    <t>file.submission_version</t>
+  </si>
+  <si>
+    <t>submission_version</t>
+  </si>
+  <si>
+    <t>study.study_version</t>
+  </si>
+  <si>
+    <t>study_version</t>
+  </si>
+  <si>
+    <t>File Version</t>
+  </si>
+  <si>
+    <t>Study Version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,13 +482,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF569CD6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEF2CD"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -476,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -488,6 +548,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C948E4-1DF0-6249-BEB1-83F763634681}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2580,6 +2644,67 @@
         <v>40</v>
       </c>
     </row>
+    <row r="85" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" t="s">
+        <v>69</v>
+      </c>
+      <c r="C85" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" t="s">
+        <v>124</v>
+      </c>
+      <c r="E85" t="str" cm="1">
+        <f t="array" ref="E85:F85">_xlfn.TEXTSPLIT(D85, ".")</f>
+        <v>file</v>
+      </c>
+      <c r="F85" t="str">
+        <v>md5sum</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86" t="s">
+        <v>130</v>
+      </c>
+      <c r="D86" t="s">
+        <v>126</v>
+      </c>
+      <c r="E86" t="s">
+        <v>42</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" t="s">
+        <v>131</v>
+      </c>
+      <c r="D87" t="s">
+        <v>128</v>
+      </c>
+      <c r="E87" t="s">
+        <v>39</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F39" xr:uid="{31C948E4-1DF0-6249-BEB1-83F763634681}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F83">
@@ -2593,10 +2718,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09E50E9-33B3-FE43-9963-D716D4024E8E}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2830,6 +2955,39 @@
         <v>120</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C18" xr:uid="{F09E50E9-33B3-FE43-9963-D716D4024E8E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
@@ -2842,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F4F2AB-5DF1-4CD4-A2B2-D6152C68451D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2886,6 +3044,14 @@
         <v>73</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>45202</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>